<commit_message>
Characters - Blue Archive - 3284538085 업데이트
</commit_message>
<xml_diff>
--- a/Data/Characters - Blue Archive - 3284538085/Characters - Blue Archive - 3284538085.xlsx
+++ b/Data/Characters - Blue Archive - 3284538085/Characters - Blue Archive - 3284538085.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Characters - Blue Archive - 3284538085\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7B9FC6-EA42-4800-B715-1C86926608C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F59CE3E-FDB5-4BE3-BB4A-00FE55CB11A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6079,12 +6079,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="E497" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-0000D2010000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-01-20에 새로 추가된 노드들 (28개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F497" authorId="0" shapeId="0" xr:uid="{CAA0369D-B01A-4389-AC59-C571BAB2A339}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-01-20에 새로 추가된 노드들 (28개)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="1762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="1869">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -6240,9 +6266,6 @@
   </si>
   <si>
     <t>BA_DisciplinaryCommitteePresident.description</t>
-  </si>
-  <si>
-    <t>{PAWN_nameDef}(은)는 모두가 두려워하는 게헨나의 선도부 부장으로, 전장에서 놀라운 위력을 발휘합니다.</t>
   </si>
   <si>
     <r>
@@ -6257,6 +6280,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>{PAWN_nameDef}(은)는 모두가 두려워하는 게헨나의 선도부 부장으로, 전장에서 놀라운 위력을 발휘합니다.</t>
+  </si>
+  <si>
     <t>BackstoryDef+BA_GourmetResearchSocietyPresident.title</t>
   </si>
   <si>
@@ -6282,9 +6308,6 @@
   </si>
   <si>
     <t>{PAWN_nameDef} is the president of the Gourmet Research Society at Gehenna Academy. Upon first look at her, one might think {PAWN_pronoun} is a rich princess-like and aloof elegance, but get her involved in talks of food and all sense of distinction is lost in this zealous gourmet.</t>
-  </si>
-  <si>
-    <t>BackstoryDef+BA_NinjutsuResearchClubMember.title</t>
   </si>
   <si>
     <r>
@@ -6299,6 +6322,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>BackstoryDef+BA_NinjutsuResearchClubMember.title</t>
+  </si>
+  <si>
     <t>BA_NinjutsuResearchClubMember.title</t>
   </si>
   <si>
@@ -10752,9 +10778,6 @@
   </si>
   <si>
     <t>KivotosStudent.description</t>
-  </si>
-  <si>
-    <t>XenotypeDef+KivotosStudent.descriptionShort</t>
   </si>
   <si>
     <r>
@@ -10781,13 +10804,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>XenotypeDef+KivotosStudent.descriptionShort</t>
+  </si>
+  <si>
     <t>KivotosStudent.descriptionShort</t>
   </si>
   <si>
     <t>The "students" of Kivotos, Which possess great physical strength and excellent attack, defense, and even regeneration abilities.</t>
-  </si>
-  <si>
-    <t>Keyed+CallRecruit</t>
   </si>
   <si>
     <r>
@@ -10802,6 +10825,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Keyed+CallRecruit</t>
+  </si>
+  <si>
     <t>Keyed</t>
   </si>
   <si>
@@ -10809,9 +10835,6 @@
   </si>
   <si>
     <t>Recruit a Blue Archive Character ({0})</t>
-  </si>
-  <si>
-    <t>Keyed+NoEnoughSilver</t>
   </si>
   <si>
     <r>
@@ -10826,13 +10849,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Keyed+NoEnoughSilver</t>
+  </si>
+  <si>
     <t>NoEnoughSilver</t>
   </si>
   <si>
     <t>Not enough silver, Need {0}</t>
-  </si>
-  <si>
-    <t>Keyed+PawnArrived</t>
   </si>
   <si>
     <r>
@@ -10847,6 +10870,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Keyed+PawnArrived</t>
+  </si>
+  <si>
     <t>PawnArrived</t>
   </si>
   <si>
@@ -10913,9 +10939,6 @@
     <t>Allow specified character recruit</t>
   </si>
   <si>
-    <t>ThingDef+Sensei_headgear.label</t>
-  </si>
-  <si>
     <t>Keyed+EnterCharacterCode</t>
   </si>
   <si>
@@ -10989,9 +11012,6 @@
   </si>
   <si>
     <t>Recruit a Blue Archive Character x10 ({0})</t>
-  </si>
-  <si>
-    <t>Keyed+BA_GachaTitle</t>
   </si>
   <si>
     <r>
@@ -11006,6 +11026,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Keyed+BA_GachaTitle</t>
+  </si>
+  <si>
     <t>BA_GachaTitle</t>
   </si>
   <si>
@@ -11121,9 +11144,6 @@
   </si>
   <si>
     <t>Ability_Shiroko_label</t>
-  </si>
-  <si>
-    <t>AbilityDef+Ability_Shiroko.description</t>
   </si>
   <si>
     <r>
@@ -11138,13 +11158,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>AbilityDef+Ability_Shiroko.description</t>
+  </si>
+  <si>
     <t>Ability_Shiroko.description</t>
   </si>
   <si>
     <t>Ability_Shiroko_description (In develop)</t>
-  </si>
-  <si>
-    <t>BackstoryDef+BA_BlackTortoisePromenadeChairman.title</t>
   </si>
   <si>
     <r>
@@ -11159,13 +11179,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>BackstoryDef+BA_BlackTortoisePromenadeChairman.title</t>
+  </si>
+  <si>
     <t>BA_BlackTortoisePromenadeChairman.title</t>
   </si>
   <si>
     <t>Black Tortoise Promenade Chairman</t>
-  </si>
-  <si>
-    <t>BackstoryDef+BA_BlackTortoisePromenadeChairman.titleShort</t>
   </si>
   <si>
     <r>
@@ -11180,13 +11200,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>BackstoryDef+BA_BlackTortoisePromenadeChairman.titleShort</t>
+  </si>
+  <si>
     <t>BA_BlackTortoisePromenadeChairman.titleShort</t>
   </si>
   <si>
     <t>Chairman</t>
-  </si>
-  <si>
-    <t>BackstoryDef+BA_BlackTortoisePromenadeChairman.description</t>
   </si>
   <si>
     <r>
@@ -11201,13 +11221,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>BackstoryDef+BA_BlackTortoisePromenadeChairman.description</t>
+  </si>
+  <si>
     <t>BA_BlackTortoisePromenadeChairman.description</t>
   </si>
   <si>
     <t>{PAWN_nameDef} is a member of Shanhaijing Senior High School and the chairman of the gourmet Black Tortoise Promenade.\nUnder {PAWN_possessive} extraordinary management, Black Tortoise Promenade grew from a mediocre shopping street into one of the best gourmet districts in Kivotos. Although {PAWN_pronoun} is at odds with the Shanhaijing student council, who are wary of {PAWN_possessive} growing influence, {PAWN_nameDef} herself seems to have no interest in anything other than developing the enterprise.</t>
-  </si>
-  <si>
-    <t>FixedPawnGenerate.FixedPawnDef+Sensei.firstName</t>
   </si>
   <si>
     <r>
@@ -11222,13 +11242,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Sensei.firstName</t>
+  </si>
+  <si>
     <t>Sensei.firstName</t>
   </si>
   <si>
     <t>Sensei</t>
-  </si>
-  <si>
-    <t>FixedPawnGenerate.FixedPawnDef+Sensei.nickName</t>
   </si>
   <si>
     <r>
@@ -11243,28 +11263,28 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Sensei.nickName</t>
+  </si>
+  <si>
     <t>Sensei.nickName</t>
   </si>
   <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Sensei.lastName</t>
+  </si>
+  <si>
     <t>Sensei.lastName</t>
   </si>
   <si>
-    <t>FixedPawnGenerate.FixedPawnDef+Sensei.lastName</t>
+    <t>HediffDef+EmptyHediff.label</t>
   </si>
   <si>
     <t>HediffDef</t>
   </si>
   <si>
-    <t>HediffDef+EmptyHediff.label</t>
-  </si>
-  <si>
     <t>EmptyHediff.label</t>
   </si>
   <si>
     <t>Empty Hediff</t>
-  </si>
-  <si>
-    <t>HediffDef+EmptyHediff.description</t>
   </si>
   <si>
     <r>
@@ -11279,13 +11299,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>HediffDef+EmptyHediff.description</t>
+  </si>
+  <si>
     <t>EmptyHediff.description</t>
   </si>
   <si>
     <t>Remove all other hediffs when generate pawn</t>
-  </si>
-  <si>
-    <t>ScenarioDef+BA_Scenario.label</t>
   </si>
   <si>
     <r>
@@ -11300,6 +11320,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ScenarioDef+BA_Scenario.label</t>
+  </si>
+  <si>
     <t>ScenarioDef</t>
   </si>
   <si>
@@ -11307,9 +11330,6 @@
   </si>
   <si>
     <t>Blue Archive Adventure</t>
-  </si>
-  <si>
-    <t>ScenarioDef+BA_Scenario.description</t>
   </si>
   <si>
     <r>
@@ -11324,13 +11344,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ScenarioDef+BA_Scenario.description</t>
+  </si>
+  <si>
     <t>BA_Scenario.description</t>
   </si>
   <si>
     <t>The spaceship crash-lands on a planet filled with mystery and danger. Resources are scarce, and the environment is harsh. As the Sensei, you must not only protect the students' safety but also guide them to find ways to survive in this unknown world. You need to use the limited resources to build shelters and explore the surroundings. The calm days won't last long, as various attacks will follow, hostile natives, ruthless mechanites, and ancient mysterious entities. \n\nEach student is unique, so take good care of them and call for support through the Comms console when necessary. \n\nNote: This is a relatively simple scenario.\n\n(It is recommended to use the Character Editor to create your own Sensei character)</t>
-  </si>
-  <si>
-    <t>ScenarioDef+BA_Scenario.scenario.summary</t>
   </si>
   <si>
     <r>
@@ -11345,13 +11365,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ScenarioDef+BA_Scenario.scenario.summary</t>
+  </si>
+  <si>
     <t>BA_Scenario.scenario.summary</t>
   </si>
   <si>
     <t>Sensei and three accompanying students from Blue Archive</t>
-  </si>
-  <si>
-    <t>ScenarioDef+BA_Scenario.scenario.name</t>
   </si>
   <si>
     <r>
@@ -11366,19 +11386,22 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ScenarioDef+BA_Scenario.scenario.name</t>
+  </si>
+  <si>
     <t>BA_Scenario.scenario.name</t>
   </si>
   <si>
+    <t>ScenarioDef+BA_Scenario.scenario.description</t>
+  </si>
+  <si>
     <t>BA_Scenario.scenario.description</t>
   </si>
   <si>
-    <t>ScenarioDef+BA_Scenario.scenario.description</t>
+    <t>ScenarioDef+BA_Scenario.scenario.parts.0.text</t>
   </si>
   <si>
     <t>BA_Scenario.scenario.parts.0.text</t>
-  </si>
-  <si>
-    <t>ScenarioDef+BA_Scenario.scenario.parts.0.text</t>
   </si>
   <si>
     <t>The sudden accident shattered the peaceful flight, and you crash-landed on a remote planet. Everything here looks so unfamiliar. The students around you gaze at you with eyes full of fear and unease. As their Sensei, you are deeply aware of the responsibility you bear. \n\nTaking a deep breath, you decide to pull yourself together and lead the students to survive.</t>
@@ -12110,9 +12133,6 @@
     <t>Gun_ShirokoDrone_Lable</t>
   </si>
   <si>
-    <t>ThingDef+Gun_ShirokoDrone.description</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -12125,13 +12145,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+Gun_ShirokoDrone.description</t>
+  </si>
+  <si>
     <t>Gun_ShirokoDrone.description</t>
   </si>
   <si>
     <t>Gun_ShirokoDrone_Description</t>
-  </si>
-  <si>
-    <t>ThingDef+Gun_ShirokoDrone.verbs.Verb_Shoot.label</t>
   </si>
   <si>
     <r>
@@ -12146,10 +12166,10 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+Gun_ShirokoDrone.verbs.Verb_Shoot.label</t>
+  </si>
+  <si>
     <t>Gun_ShirokoDrone.verbs.Verb_Shoot.label</t>
-  </si>
-  <si>
-    <t>FixedPawnGenerate.FixedPawnDef+Arisu.firstName</t>
   </si>
   <si>
     <r>
@@ -12164,13 +12184,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Arisu.firstName</t>
+  </si>
+  <si>
     <t>Arisu.firstName</t>
   </si>
   <si>
     <t>Arisu</t>
-  </si>
-  <si>
-    <t>FixedPawnGenerate.FixedPawnDef+Arisu.nickName</t>
   </si>
   <si>
     <r>
@@ -12185,19 +12205,19 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Arisu.nickName</t>
+  </si>
+  <si>
     <t>Arisu.nickName</t>
   </si>
   <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Arisu.lastName</t>
+  </si>
+  <si>
     <t>Arisu.lastName</t>
   </si>
   <si>
-    <t>FixedPawnGenerate.FixedPawnDef+Arisu.lastName</t>
-  </si>
-  <si>
     <t>Tendou</t>
-  </si>
-  <si>
-    <t>FixedPawnGenerate.FixedPawnDef+Rumi.firstName</t>
   </si>
   <si>
     <r>
@@ -12212,13 +12232,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Rumi.firstName</t>
+  </si>
+  <si>
     <t>Rumi.firstName</t>
   </si>
   <si>
     <t>Rumi</t>
-  </si>
-  <si>
-    <t>FixedPawnGenerate.FixedPawnDef+Rumi.nickName</t>
   </si>
   <si>
     <r>
@@ -12233,19 +12253,19 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Rumi.nickName</t>
+  </si>
+  <si>
     <t>Rumi.nickName</t>
   </si>
   <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Rumi.lastName</t>
+  </si>
+  <si>
     <t>Rumi.lastName</t>
   </si>
   <si>
-    <t>FixedPawnGenerate.FixedPawnDef+Rumi.lastName</t>
-  </si>
-  <si>
     <t>Akeshiro</t>
-  </si>
-  <si>
-    <t>Sensei_headgear.label</t>
   </si>
   <si>
     <r>
@@ -12260,24 +12280,54 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+Sensei_headgear.label</t>
+  </si>
+  <si>
+    <t>Sensei_headgear.label</t>
+  </si>
+  <si>
     <t>Sensei headgear</t>
   </si>
   <si>
     <t>ThingDef+Sensei_headgear.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>(블루 아카이브) 선생 머리장식</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Sensei_headgear.description</t>
   </si>
   <si>
+    <t>BA_allowSpecifieSpawn</t>
+  </si>
+  <si>
     <t>Keyed+BA_allowSpecifieSpawn</t>
   </si>
   <si>
-    <t>BA_allowSpecifieSpawn</t>
-  </si>
-  <si>
     <t>Keyed+BA_allowSpecifieSpawn_description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>지정 캐릭터 모집 허용</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BA_allowSpecifieSpawn_description</t>
   </si>
   <si>
@@ -12287,6 +12337,18 @@
     <t>Keyed+BA_senseiTexturePath</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>은 10,000개를 소모해 지정한 캐릭터를 모집합니다. 캐릭터의 영어 이름을 입력해야 합니다. 자세한 네용은 영어 위키를 참고하세요.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BA_senseiTexturePath</t>
   </si>
   <si>
@@ -12296,29 +12358,381 @@
     <t>Keyed+BA_senseiTexturePath_description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>선생 초상화 파일 경로</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BA_senseiTexturePath_description</t>
   </si>
   <si>
     <t>Must use absolute path</t>
   </si>
   <si>
-    <t>(블루 아카이브) 선생 머리장식</t>
+    <t>BackstoryDef+BA_SweetsClubTroublemaker.title</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>전체 경로를 입력해야 합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>BA_SweetsClubTroublemaker.title</t>
+  </si>
+  <si>
+    <t>After-School Sweets Club Troublemaker</t>
+  </si>
+  <si>
+    <t>BackstoryDef+BA_SweetsClubTroublemaker.titleShort</t>
+  </si>
+  <si>
+    <t>BA_SweetsClubTroublemaker.titleShort</t>
+  </si>
+  <si>
+    <t>Troublemaker</t>
+  </si>
+  <si>
+    <t>BackstoryDef+BA_SweetsClubTroublemaker.description</t>
+  </si>
+  <si>
+    <t>BA_SweetsClubTroublemaker.description</t>
+  </si>
+  <si>
+    <t>BackstoryDef+BA_EngineeringClubLeader.title</t>
+  </si>
+  <si>
+    <t>BA_EngineeringClubLeader.title</t>
+  </si>
+  <si>
+    <t>Engineering Club Leader</t>
+  </si>
+  <si>
+    <t>BackstoryDef+BA_EngineeringClubLeader.titleShort</t>
+  </si>
+  <si>
+    <t>BA_EngineeringClubLeader.titleShort</t>
+  </si>
+  <si>
+    <t>Leader</t>
+  </si>
+  <si>
+    <t>BackstoryDef+BA_EngineeringClubLeader.description</t>
+  </si>
+  <si>
+    <t>BA_EngineeringClubLeader.description</t>
+  </si>
+  <si>
+    <t>ThoughtDef+BA_Romanticist.stages.0.label</t>
+  </si>
+  <si>
+    <t>ThoughtDef</t>
+  </si>
+  <si>
+    <t>BA_Romanticist.stages.0.label</t>
+  </si>
+  <si>
+    <t>romanticist</t>
+  </si>
+  <si>
+    <t>ThoughtDef+BA_RomanticistPresence.stages.0.label</t>
+  </si>
+  <si>
+    <t>Romanticist presence</t>
+  </si>
+  <si>
+    <t>ThoughtDef+BA_RomanticistPresence.stages.0.description</t>
+  </si>
+  <si>
+    <t>BA_RomanticistPresence.stages.0.description</t>
+  </si>
+  <si>
+    <t>I felt the beauty and poetry of life in this colony, as if everything became more beautiful.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+BA_Sensei.stages.0.label</t>
+  </si>
+  <si>
+    <t>BA_Sensei.stages.0.label</t>
+  </si>
+  <si>
+    <t>sensei</t>
+  </si>
+  <si>
+    <t>ThoughtDef+BA_SenseiPresence.stages.0.label</t>
+  </si>
+  <si>
+    <t>BA_SenseiPresence.stages.0.label</t>
+  </si>
+  <si>
+    <t>Sensei presence</t>
+  </si>
+  <si>
+    <t>ThoughtDef+BA_SenseiPresence.stages.0.description</t>
+  </si>
+  <si>
+    <t>BA_SenseiPresence.stages.0.description</t>
+  </si>
+  <si>
+    <t>Sensei is right next to me, I'm so happy.</t>
+  </si>
+  <si>
+    <t>TraitDef+BA_Sensei.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>BA_Sensei.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>Kivotos sensei</t>
+  </si>
+  <si>
+    <t>TraitDef+BA_Sensei.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>BA_Sensei.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}is the Kivotos sensei deeply loved by the students.</t>
+  </si>
+  <si>
+    <t>TraitDef+BA_Romanticist.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>BA_Romanticist.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>TraitDef+BA_Romanticist.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>BA_Romanticist.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}is a firm believer in romanticism and often describes every detail of life in poetic language. {PAWN_pronoun} presence brings a romantic atmosphere to those around her.</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Utaha.firstName</t>
+  </si>
+  <si>
+    <t>Utaha.firstName</t>
+  </si>
+  <si>
+    <t>Utaha</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Utaha.nickName</t>
+  </si>
+  <si>
+    <t>Utaha.nickName</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Utaha.lastName</t>
+  </si>
+  <si>
+    <t>Utaha.lastName</t>
+  </si>
+  <si>
+    <t>Shiraishi</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Natsu.firstName</t>
+  </si>
+  <si>
+    <t>Natsu.firstName</t>
+  </si>
+  <si>
+    <t>Natsu</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Natsu.nickName</t>
+  </si>
+  <si>
+    <t>Natsu.nickName</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+Natsu.lastName</t>
+  </si>
+  <si>
+    <t>Natsu.lastName</t>
+  </si>
+  <si>
+    <t>Yutori</t>
+  </si>
+  <si>
+    <t>Keyed+BA_senseiPortraitOffsetX</t>
+  </si>
+  <si>
+    <t>BA_senseiPortraitOffsetX</t>
+  </si>
+  <si>
+    <t>Offset X</t>
+  </si>
+  <si>
+    <t>Keyed+BA_senseiPortraitOffsetX_description</t>
+  </si>
+  <si>
+    <t>BA_senseiPortraitOffsetX_description</t>
+  </si>
+  <si>
+    <t>Horizontal offset</t>
+  </si>
+  <si>
+    <t>Keyed+BA_senseiPortraitOffsetY</t>
+  </si>
+  <si>
+    <t>BA_senseiPortraitOffsetY</t>
+  </si>
+  <si>
+    <t>Offset Y</t>
+  </si>
+  <si>
+    <t>Keyed+BA_senseiPortraitOffsetYBuffer_description</t>
+  </si>
+  <si>
+    <t>BA_senseiPortraitOffsetYBuffer_description</t>
+  </si>
+  <si>
+    <t>Vertical offset</t>
+  </si>
+  <si>
+    <t>Keyed+BA_senseiPortraitScale</t>
+  </si>
+  <si>
+    <t>BA_senseiPortraitScale</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Keyed+BA_senseiPortraitScaleBuffer_description</t>
+  </si>
+  <si>
+    <t>BA_senseiPortraitScaleBuffer_description</t>
+  </si>
+  <si>
+    <t>Scale of the picture</t>
+  </si>
+  <si>
+    <t>방과후 디저트부 트러블 메이커</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>전체 경로를 입력해야 합니다.</t>
+    <t>트러블 메이커</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef} is a student of Trinity Integrated Academy, {PAWN_nameDef} is the chief troublemaker of the After School Sweets Club and a self-described romanticist.\n\n{PAWN_nameDef} has a habit of saying philosophical things out of the blue and using sweets as a metaphor. While {PAWN_possessive} erratic outbursts always leave everyone bamboozled, in reality {PAWN_pronoun} simply has the pure intention of wanting to share in the romanticism with everyone. Unfortunately {PAWN_possessive} constantly changing definition of "romanticism" leaves others with the undeniable impression that they're just being messed around with.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>선생 초상화 파일 경로</t>
+    <t>{PAWN_nameDef}(은)는 트리니티 트리니티 방과후 디저트부 소속의 일원으로, 트러블 메이커의 필두이자 자칭 로맨티스트입니다.\n\n{PAWN_pronoun}(은)는 묘하게 철학적인 말을 하거나, 만사를 디저트에 빗대어 표현하는 버릇이 있습니다. 늘 엉뚱한 일로 주변을 곤란하게 만들지만, 이는 모두와 함께 로망을 공유하고 싶다는 순수한 마음 때문입니다. 하지만 {PAWN_pronoun}(이)가 이야기하는 로망의 정의가 항상 바뀌기 때문에, 옆에서 보면 모두가 나츠에게 휘둘리고 있다는 인상을 부정할 순 없습니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>지정 캐릭터 모집 허용</t>
+    <t>엔지니어부 부장</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>은 10,000개를 소모해 지정한 캐릭터를 모집합니다. 캐릭터의 영어 이름을 입력해야 합니다. 자세한 네용은 영어 위키를 참고하세요.</t>
+    <t>부장</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{PAWN_nameDef} is the club leader of the Engineering Club at Millennium Science School.\n\nWithout straying from that title, {PAWN_nameDef} continues to develop all sorts of various robots. One {PAWN_pronoun} always brings along, Rai-chan, is known for having capabilities that can rival several hundred PMC Automata.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 밀레니엄 학원 엔지니어부의 부장입니다.\n\n{PAWN_nameDef}(은)는 엔지니어부의 부장이라는 직함을 증명이라도 하듯 다양한 로봇을 발명하였으며, 특히 {PAWN_pronoun}의 애완로봇 "천둥이"는 PMC의 전투용 오토마타 수백 대에 달하는 전투 능력을 갖추었다고 평가받고 있습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>로맨티스트</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BA_RomanticistPresence.stages.0.label</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>로맨티스트 존재</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>선생 존재</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>이곳에서 삶의 아름다움과 현학적인 감상이 느껴져. 모든 것이 한층 아름답게 변한 것 같아.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>선생님과 함께함</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>선생님이 곁에 계셔서 너무 기뻐.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 학생들에게 사랑받는 키보토스의 선생입니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 로망을 위해서라면 무슨 일이든 합니다.  {PAWN_pronoun}의 존재는 주변 사람들에게 낭만적인 분위기를 가져다줍니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>우타하</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>시라이시</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>나츠</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>유토리</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>크기</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y축</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X축</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수평 위치를 조절합니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수직 위치를 조절합니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>그림 크기를 조절합니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>샬레 선생</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -12721,10 +13135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F496"/>
+  <dimension ref="A1:F524"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A474" workbookViewId="0">
-      <selection activeCell="F494" sqref="F494"/>
+    <sheetView tabSelected="1" topLeftCell="A492" workbookViewId="0">
+      <selection activeCell="F510" sqref="F510"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17"/>
@@ -12951,10 +13365,10 @@
         <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -13005,12 +13419,12 @@
         <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
@@ -20178,15 +20592,15 @@
         <v>1549</v>
       </c>
       <c r="E439" s="2" t="s">
+        <v>1550</v>
+      </c>
+      <c r="F439" s="1" t="s">
         <v>1551</v>
-      </c>
-      <c r="F439" s="1" t="s">
-        <v>1552</v>
       </c>
     </row>
     <row r="440" spans="1:6">
       <c r="A440" s="1" t="s">
-        <v>1550</v>
+        <v>1552</v>
       </c>
       <c r="B440" s="1" t="s">
         <v>1546</v>
@@ -20198,12 +20612,12 @@
         <v>1554</v>
       </c>
       <c r="F440" s="1" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="441" spans="1:6">
       <c r="A441" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="B441" s="1" t="s">
         <v>1557</v>
@@ -20215,12 +20629,12 @@
         <v>1559</v>
       </c>
       <c r="F441" s="1" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="442" spans="1:6">
       <c r="A442" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="B442" s="1" t="s">
         <v>1557</v>
@@ -20232,12 +20646,12 @@
         <v>1563</v>
       </c>
       <c r="F442" s="1" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="443" spans="1:6">
       <c r="A443" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="B443" s="1" t="s">
         <v>1557</v>
@@ -20336,64 +20750,64 @@
     </row>
     <row r="449" spans="1:6">
       <c r="A449" s="1" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B449" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C449" s="1" t="s">
+        <v>1589</v>
+      </c>
+      <c r="E449" s="2" t="s">
         <v>1590</v>
       </c>
-      <c r="E449" s="2" t="s">
+      <c r="F449" s="1" t="s">
         <v>1591</v>
-      </c>
-      <c r="F449" s="1" t="s">
-        <v>1592</v>
       </c>
     </row>
     <row r="450" spans="1:6">
       <c r="A450" s="1" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B450" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C450" s="1" t="s">
+        <v>1593</v>
+      </c>
+      <c r="E450" s="2" t="s">
         <v>1594</v>
       </c>
-      <c r="E450" s="2" t="s">
+      <c r="F450" s="1" t="s">
         <v>1595</v>
-      </c>
-      <c r="F450" s="1" t="s">
-        <v>1596</v>
       </c>
     </row>
     <row r="451" spans="1:6">
       <c r="A451" s="1" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="B451" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C451" s="1" t="s">
+        <v>1597</v>
+      </c>
+      <c r="E451" s="2" t="s">
         <v>1598</v>
       </c>
-      <c r="E451" s="2" t="s">
+      <c r="F451" s="1" t="s">
         <v>1599</v>
-      </c>
-      <c r="F451" s="1" t="s">
-        <v>1600</v>
       </c>
     </row>
     <row r="452" spans="1:6">
       <c r="A452" s="1" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="B452" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C452" s="1" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="E452" s="2" t="s">
         <v>1567</v>
@@ -20404,53 +20818,53 @@
     </row>
     <row r="453" spans="1:6">
       <c r="A453" s="1" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="B453" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C453" s="1" t="s">
+        <v>1603</v>
+      </c>
+      <c r="E453" s="2" t="s">
         <v>1604</v>
       </c>
-      <c r="E453" s="2" t="s">
+      <c r="F453" s="1" t="s">
         <v>1605</v>
-      </c>
-      <c r="F453" s="1" t="s">
-        <v>1606</v>
       </c>
     </row>
     <row r="454" spans="1:6">
       <c r="A454" s="1" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="B454" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C454" s="1" t="s">
+        <v>1607</v>
+      </c>
+      <c r="E454" s="2" t="s">
         <v>1608</v>
       </c>
-      <c r="E454" s="2" t="s">
+      <c r="F454" s="1" t="s">
         <v>1609</v>
-      </c>
-      <c r="F454" s="1" t="s">
-        <v>1610</v>
       </c>
     </row>
     <row r="455" spans="1:6">
       <c r="A455" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="B455" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C455" s="1" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E455" s="2" t="s">
         <v>1612</v>
       </c>
-      <c r="E455" s="2" t="s">
+      <c r="F455" s="1" t="s">
         <v>1613</v>
-      </c>
-      <c r="F455" s="1" t="s">
-        <v>1615</v>
       </c>
     </row>
     <row r="456" spans="1:6">
@@ -20461,166 +20875,166 @@
         <v>1557</v>
       </c>
       <c r="C456" s="1" t="s">
+        <v>1615</v>
+      </c>
+      <c r="E456" s="2" t="s">
         <v>1616</v>
       </c>
-      <c r="E456" s="2" t="s">
+      <c r="F456" s="1" t="s">
         <v>1617</v>
-      </c>
-      <c r="F456" s="1" t="s">
-        <v>1618</v>
       </c>
     </row>
     <row r="457" spans="1:6">
       <c r="A457" s="1" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="B457" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C457" s="1" t="s">
+        <v>1619</v>
+      </c>
+      <c r="E457" s="2" t="s">
         <v>1620</v>
       </c>
-      <c r="E457" s="2" t="s">
+      <c r="F457" s="1" t="s">
         <v>1621</v>
-      </c>
-      <c r="F457" s="1" t="s">
-        <v>1622</v>
       </c>
     </row>
     <row r="458" spans="1:6">
       <c r="A458" s="1" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B458" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C458" s="1" t="s">
+        <v>1623</v>
+      </c>
+      <c r="E458" s="2" t="s">
         <v>1624</v>
       </c>
-      <c r="E458" s="2" t="s">
+      <c r="F458" s="1" t="s">
         <v>1625</v>
-      </c>
-      <c r="F458" s="1" t="s">
-        <v>1626</v>
       </c>
     </row>
     <row r="459" spans="1:6">
       <c r="A459" s="1" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="B459" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C459" s="1" t="s">
+        <v>1627</v>
+      </c>
+      <c r="E459" s="2" t="s">
         <v>1628</v>
       </c>
-      <c r="E459" s="2" t="s">
+      <c r="F459" s="1" t="s">
         <v>1629</v>
-      </c>
-      <c r="F459" s="1" t="s">
-        <v>1630</v>
       </c>
     </row>
     <row r="460" spans="1:6">
       <c r="A460" s="1" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="B460" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C460" s="1" t="s">
+        <v>1631</v>
+      </c>
+      <c r="E460" s="2" t="s">
         <v>1632</v>
       </c>
-      <c r="E460" s="2" t="s">
+      <c r="F460" s="1" t="s">
         <v>1633</v>
-      </c>
-      <c r="F460" s="1" t="s">
-        <v>1634</v>
       </c>
     </row>
     <row r="461" spans="1:6">
       <c r="A461" s="1" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="B461" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C461" s="1" t="s">
+        <v>1635</v>
+      </c>
+      <c r="E461" s="2" t="s">
         <v>1636</v>
       </c>
-      <c r="E461" s="2" t="s">
+      <c r="F461" s="1" t="s">
         <v>1637</v>
-      </c>
-      <c r="F461" s="1" t="s">
-        <v>1638</v>
       </c>
     </row>
     <row r="462" spans="1:6">
       <c r="A462" s="1" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B462" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C462" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="E462" s="2" t="s">
         <v>1640</v>
       </c>
-      <c r="E462" s="2" t="s">
+      <c r="F462" s="1" t="s">
         <v>1641</v>
-      </c>
-      <c r="F462" s="1" t="s">
-        <v>1642</v>
       </c>
     </row>
     <row r="463" spans="1:6">
       <c r="A463" s="1" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="B463" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C463" s="1" t="s">
+        <v>1643</v>
+      </c>
+      <c r="E463" s="2" t="s">
         <v>1644</v>
       </c>
-      <c r="E463" s="2" t="s">
+      <c r="F463" s="1" t="s">
         <v>1645</v>
-      </c>
-      <c r="F463" s="1" t="s">
-        <v>1646</v>
       </c>
     </row>
     <row r="464" spans="1:6">
       <c r="A464" s="1" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="B464" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C464" s="1" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E464" s="2" t="s">
         <v>1648</v>
       </c>
-      <c r="E464" s="2" t="s">
+      <c r="F464" s="1" t="s">
         <v>1649</v>
-      </c>
-      <c r="F464" s="1" t="s">
-        <v>1650</v>
       </c>
     </row>
     <row r="466" spans="1:6">
       <c r="A466" s="1" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B466" s="1" t="s">
         <v>1651</v>
       </c>
-      <c r="B466" s="1" t="s">
+      <c r="C466" s="1" t="s">
         <v>1652</v>
       </c>
-      <c r="C466" s="1" t="s">
+      <c r="E466" s="4" t="s">
         <v>1653</v>
       </c>
-      <c r="E466" s="4" t="s">
+      <c r="F466" s="1" t="s">
         <v>1654</v>
-      </c>
-      <c r="F466" s="1" t="s">
-        <v>1656</v>
       </c>
     </row>
     <row r="467" spans="1:6">
@@ -20628,16 +21042,16 @@
         <v>1655</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="C467" s="1" t="s">
+        <v>1656</v>
+      </c>
+      <c r="E467" s="1" t="s">
         <v>1657</v>
       </c>
-      <c r="E467" s="1" t="s">
+      <c r="F467" s="1" t="s">
         <v>1658</v>
-      </c>
-      <c r="F467" s="1" t="s">
-        <v>1660</v>
       </c>
     </row>
     <row r="468" spans="1:6">
@@ -20648,13 +21062,13 @@
         <v>7</v>
       </c>
       <c r="C468" s="1" t="s">
+        <v>1660</v>
+      </c>
+      <c r="E468" s="1" t="s">
         <v>1661</v>
       </c>
-      <c r="E468" s="1" t="s">
+      <c r="F468" s="1" t="s">
         <v>1662</v>
-      </c>
-      <c r="F468" s="1" t="s">
-        <v>1664</v>
       </c>
     </row>
     <row r="469" spans="1:6">
@@ -20665,13 +21079,13 @@
         <v>7</v>
       </c>
       <c r="C469" s="1" t="s">
+        <v>1664</v>
+      </c>
+      <c r="E469" s="1" t="s">
         <v>1665</v>
       </c>
-      <c r="E469" s="1" t="s">
+      <c r="F469" s="1" t="s">
         <v>1666</v>
-      </c>
-      <c r="F469" s="1" t="s">
-        <v>1668</v>
       </c>
     </row>
     <row r="470" spans="1:6">
@@ -20682,13 +21096,13 @@
         <v>7</v>
       </c>
       <c r="C470" s="1" t="s">
+        <v>1668</v>
+      </c>
+      <c r="E470" s="1" t="s">
         <v>1669</v>
       </c>
-      <c r="E470" s="1" t="s">
+      <c r="F470" s="1" t="s">
         <v>1670</v>
-      </c>
-      <c r="F470" s="1" t="s">
-        <v>1672</v>
       </c>
     </row>
     <row r="471" spans="1:6">
@@ -20699,13 +21113,13 @@
         <v>665</v>
       </c>
       <c r="C471" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="E471" s="1" t="s">
         <v>1673</v>
       </c>
-      <c r="E471" s="1" t="s">
+      <c r="F471" s="1" t="s">
         <v>1674</v>
-      </c>
-      <c r="F471" s="1" t="s">
-        <v>1676</v>
       </c>
     </row>
     <row r="472" spans="1:6">
@@ -20716,18 +21130,18 @@
         <v>665</v>
       </c>
       <c r="C472" s="1" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="E472" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="F472" s="1" t="s">
         <v>1674</v>
-      </c>
-      <c r="F472" s="1" t="s">
-        <v>1676</v>
       </c>
     </row>
     <row r="473" spans="1:6">
       <c r="A473" s="1" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="B473" s="1" t="s">
         <v>665</v>
@@ -20736,27 +21150,27 @@
         <v>1678</v>
       </c>
       <c r="E473" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="F473" s="1" t="s">
         <v>1674</v>
-      </c>
-      <c r="F473" s="1" t="s">
-        <v>1676</v>
       </c>
     </row>
     <row r="474" spans="1:6">
       <c r="A474" s="1" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="B474" s="1" t="s">
         <v>1680</v>
       </c>
       <c r="C474" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E474" s="1" t="s">
         <v>1682</v>
       </c>
-      <c r="E474" s="1" t="s">
+      <c r="F474" s="1" t="s">
         <v>1683</v>
-      </c>
-      <c r="F474" s="1" t="s">
-        <v>1685</v>
       </c>
     </row>
     <row r="475" spans="1:6">
@@ -20767,13 +21181,13 @@
         <v>1680</v>
       </c>
       <c r="C475" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="E475" s="1" t="s">
         <v>1686</v>
       </c>
-      <c r="E475" s="1" t="s">
+      <c r="F475" s="1" t="s">
         <v>1687</v>
-      </c>
-      <c r="F475" s="1" t="s">
-        <v>1689</v>
       </c>
     </row>
     <row r="476" spans="1:6">
@@ -20781,16 +21195,16 @@
         <v>1688</v>
       </c>
       <c r="B476" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C476" s="1" t="s">
         <v>1690</v>
       </c>
-      <c r="C476" s="1" t="s">
+      <c r="E476" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="E476" s="1" t="s">
+      <c r="F476" s="1" t="s">
         <v>1692</v>
-      </c>
-      <c r="F476" s="1" t="s">
-        <v>1694</v>
       </c>
     </row>
     <row r="477" spans="1:6">
@@ -20798,16 +21212,16 @@
         <v>1693</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="C477" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="E477" s="1" t="s">
         <v>1695</v>
       </c>
-      <c r="E477" s="1" t="s">
+      <c r="F477" s="1" t="s">
         <v>1696</v>
-      </c>
-      <c r="F477" s="1" t="s">
-        <v>1698</v>
       </c>
     </row>
     <row r="478" spans="1:6">
@@ -20815,16 +21229,16 @@
         <v>1697</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="C478" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="E478" s="1" t="s">
         <v>1699</v>
       </c>
-      <c r="E478" s="1" t="s">
+      <c r="F478" s="1" t="s">
         <v>1700</v>
-      </c>
-      <c r="F478" s="1" t="s">
-        <v>1702</v>
       </c>
     </row>
     <row r="479" spans="1:6">
@@ -20832,67 +21246,67 @@
         <v>1701</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="C479" s="1" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="E479" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="F479" s="1" t="s">
         <v>1692</v>
-      </c>
-      <c r="F479" s="1" t="s">
-        <v>1694</v>
       </c>
     </row>
     <row r="480" spans="1:6">
       <c r="A480" s="1" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="C480" s="1" t="s">
         <v>1704</v>
       </c>
       <c r="E480" s="1" t="s">
+        <v>1695</v>
+      </c>
+      <c r="F480" s="1" t="s">
         <v>1696</v>
-      </c>
-      <c r="F480" s="1" t="s">
-        <v>1698</v>
       </c>
     </row>
     <row r="481" spans="1:6">
       <c r="A481" s="1" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="C481" s="1" t="s">
         <v>1706</v>
       </c>
       <c r="E481" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="F481" s="5" t="s">
         <v>1708</v>
-      </c>
-      <c r="F481" s="5" t="s">
-        <v>1709</v>
       </c>
     </row>
     <row r="482" spans="1:6">
       <c r="A482" s="1" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B482" s="1" t="s">
         <v>1710</v>
       </c>
-      <c r="B482" s="1" t="s">
+      <c r="C482" s="1" t="s">
         <v>1711</v>
       </c>
-      <c r="C482" s="1" t="s">
+      <c r="E482" s="1" t="s">
         <v>1712</v>
       </c>
-      <c r="E482" s="1" t="s">
+      <c r="F482" s="1" t="s">
         <v>1713</v>
-      </c>
-      <c r="F482" s="1" t="s">
-        <v>1715</v>
       </c>
     </row>
     <row r="483" spans="1:6">
@@ -20900,16 +21314,16 @@
         <v>1714</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="C483" s="1" t="s">
+        <v>1715</v>
+      </c>
+      <c r="E483" s="1" t="s">
         <v>1716</v>
       </c>
-      <c r="E483" s="1" t="s">
+      <c r="F483" s="1" t="s">
         <v>1717</v>
-      </c>
-      <c r="F483" s="1" t="s">
-        <v>1719</v>
       </c>
     </row>
     <row r="484" spans="1:6">
@@ -20917,16 +21331,16 @@
         <v>1718</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="C484" s="1" t="s">
+        <v>1719</v>
+      </c>
+      <c r="E484" s="1" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F484" s="1" t="s">
         <v>1720</v>
-      </c>
-      <c r="E484" s="1" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F484" s="1" t="s">
-        <v>1722</v>
       </c>
     </row>
     <row r="485" spans="1:6">
@@ -20937,13 +21351,13 @@
         <v>665</v>
       </c>
       <c r="C485" s="1" t="s">
+        <v>1722</v>
+      </c>
+      <c r="E485" s="1" t="s">
         <v>1723</v>
       </c>
-      <c r="E485" s="1" t="s">
+      <c r="F485" s="1" t="s">
         <v>1724</v>
-      </c>
-      <c r="F485" s="1" t="s">
-        <v>1726</v>
       </c>
     </row>
     <row r="486" spans="1:6">
@@ -20954,18 +21368,18 @@
         <v>665</v>
       </c>
       <c r="C486" s="1" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="E486" s="1" t="s">
+        <v>1723</v>
+      </c>
+      <c r="F486" s="1" t="s">
         <v>1724</v>
-      </c>
-      <c r="F486" s="1" t="s">
-        <v>1726</v>
       </c>
     </row>
     <row r="487" spans="1:6">
       <c r="A487" s="1" t="s">
-        <v>1729</v>
+        <v>1727</v>
       </c>
       <c r="B487" s="1" t="s">
         <v>665</v>
@@ -20974,10 +21388,10 @@
         <v>1728</v>
       </c>
       <c r="E487" s="1" t="s">
+        <v>1729</v>
+      </c>
+      <c r="F487" s="1" t="s">
         <v>1730</v>
-      </c>
-      <c r="F487" s="1" t="s">
-        <v>1732</v>
       </c>
     </row>
     <row r="488" spans="1:6">
@@ -20988,13 +21402,13 @@
         <v>665</v>
       </c>
       <c r="C488" s="1" t="s">
+        <v>1732</v>
+      </c>
+      <c r="E488" s="1" t="s">
         <v>1733</v>
       </c>
-      <c r="E488" s="1" t="s">
+      <c r="F488" s="1" t="s">
         <v>1734</v>
-      </c>
-      <c r="F488" s="1" t="s">
-        <v>1736</v>
       </c>
     </row>
     <row r="489" spans="1:6">
@@ -21005,18 +21419,18 @@
         <v>665</v>
       </c>
       <c r="C489" s="1" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="E489" s="1" t="s">
+        <v>1733</v>
+      </c>
+      <c r="F489" s="1" t="s">
         <v>1734</v>
-      </c>
-      <c r="F489" s="1" t="s">
-        <v>1736</v>
       </c>
     </row>
     <row r="490" spans="1:6">
       <c r="A490" s="1" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="B490" s="1" t="s">
         <v>665</v>
@@ -21025,27 +21439,27 @@
         <v>1738</v>
       </c>
       <c r="E490" s="1" t="s">
+        <v>1739</v>
+      </c>
+      <c r="F490" s="1" t="s">
         <v>1740</v>
-      </c>
-      <c r="F490" s="1" t="s">
-        <v>1742</v>
       </c>
     </row>
     <row r="491" spans="1:6">
       <c r="A491" s="1" t="s">
-        <v>1588</v>
+        <v>1741</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="C491" s="1" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="E491" s="4" t="s">
         <v>1743</v>
       </c>
       <c r="F491" s="1" t="s">
-        <v>1757</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="492" spans="1:6">
@@ -21053,21 +21467,21 @@
         <v>1744</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="C492" s="1" t="s">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="E492" s="1" t="s">
         <v>1743</v>
       </c>
       <c r="F492" s="1" t="s">
-        <v>1757</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="493" spans="1:6">
       <c r="A493" s="1" t="s">
-        <v>1746</v>
+        <v>1748</v>
       </c>
       <c r="B493" s="1" t="s">
         <v>1557</v>
@@ -21079,58 +21493,534 @@
         <v>1587</v>
       </c>
       <c r="F493" s="1" t="s">
-        <v>1760</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="494" spans="1:6">
       <c r="A494" s="1" t="s">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="B494" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C494" s="1" t="s">
-        <v>1749</v>
+        <v>1751</v>
       </c>
       <c r="E494" s="1" t="s">
-        <v>1750</v>
+        <v>1752</v>
       </c>
       <c r="F494" s="1" t="s">
-        <v>1761</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="495" spans="1:6">
       <c r="A495" s="1" t="s">
-        <v>1751</v>
+        <v>1753</v>
       </c>
       <c r="B495" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C495" s="1" t="s">
-        <v>1752</v>
+        <v>1755</v>
       </c>
       <c r="E495" s="1" t="s">
-        <v>1753</v>
+        <v>1756</v>
       </c>
       <c r="F495" s="1" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="496" spans="1:6">
       <c r="A496" s="1" t="s">
-        <v>1754</v>
+        <v>1757</v>
       </c>
       <c r="B496" s="1" t="s">
         <v>1557</v>
       </c>
       <c r="C496" s="1" t="s">
-        <v>1755</v>
+        <v>1759</v>
       </c>
       <c r="E496" s="1" t="s">
-        <v>1756</v>
+        <v>1760</v>
       </c>
       <c r="F496" s="1" t="s">
-        <v>1758</v>
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6">
+      <c r="A497" s="1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C497" s="1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="E497" s="4" t="s">
+        <v>1764</v>
+      </c>
+      <c r="F497" s="4" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6">
+      <c r="A498" s="1" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C498" s="1" t="s">
+        <v>1766</v>
+      </c>
+      <c r="E498" s="1" t="s">
+        <v>1767</v>
+      </c>
+      <c r="F498" s="1" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6">
+      <c r="A499" s="1" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C499" s="1" t="s">
+        <v>1769</v>
+      </c>
+      <c r="E499" s="1" t="s">
+        <v>1843</v>
+      </c>
+      <c r="F499" s="1" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6">
+      <c r="A500" s="1" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C500" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="E500" s="1" t="s">
+        <v>1772</v>
+      </c>
+      <c r="F500" s="1" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="501" spans="1:6">
+      <c r="A501" s="1" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C501" s="1" t="s">
+        <v>1774</v>
+      </c>
+      <c r="E501" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="F501" s="1" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="502" spans="1:6">
+      <c r="A502" s="1" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C502" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="E502" s="1" t="s">
+        <v>1847</v>
+      </c>
+      <c r="F502" s="1" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6">
+      <c r="A503" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C503" s="1" t="s">
+        <v>1780</v>
+      </c>
+      <c r="E503" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="F503" s="1" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6">
+      <c r="A504" s="1" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C504" s="1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="E504" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="F504" s="1" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6">
+      <c r="A505" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C505" s="1" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E505" s="1" t="s">
+        <v>1786</v>
+      </c>
+      <c r="F505" s="1" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6">
+      <c r="A506" s="1" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C506" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="E506" s="1" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F506" s="1" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6">
+      <c r="A507" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C507" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="E507" s="1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="F507" s="1" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6">
+      <c r="A508" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C508" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="E508" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="F508" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6">
+      <c r="A509" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C509" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="E509" s="1" t="s">
+        <v>1798</v>
+      </c>
+      <c r="F509" s="1" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6">
+      <c r="A510" s="1" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C510" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="E510" s="1" t="s">
+        <v>1801</v>
+      </c>
+      <c r="F510" s="1" t="s">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6">
+      <c r="A511" s="1" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C511" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="E511" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="F511" s="1" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6">
+      <c r="A512" s="1" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C512" s="1" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E512" s="1" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F512" s="1" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6">
+      <c r="A513" s="1" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C513" s="1" t="s">
+        <v>1808</v>
+      </c>
+      <c r="E513" s="1" t="s">
+        <v>1809</v>
+      </c>
+      <c r="F513" s="1" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6">
+      <c r="A514" s="1" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C514" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="E514" s="1" t="s">
+        <v>1809</v>
+      </c>
+      <c r="F514" s="1" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6">
+      <c r="A515" s="1" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C515" s="1" t="s">
+        <v>1813</v>
+      </c>
+      <c r="E515" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="F515" s="1" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6">
+      <c r="A516" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C516" s="1" t="s">
+        <v>1816</v>
+      </c>
+      <c r="E516" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="F516" s="1" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6">
+      <c r="A517" s="1" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C517" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E517" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="F517" s="1" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6">
+      <c r="A518" s="1" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C518" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="E518" s="1" t="s">
+        <v>1822</v>
+      </c>
+      <c r="F518" s="1" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6">
+      <c r="A519" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C519" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="E519" s="1" t="s">
+        <v>1825</v>
+      </c>
+      <c r="F519" s="1" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6">
+      <c r="A520" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C520" s="1" t="s">
+        <v>1827</v>
+      </c>
+      <c r="E520" s="1" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F520" s="1" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6">
+      <c r="A521" s="1" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C521" s="1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="E521" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="F521" s="1" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6">
+      <c r="A522" s="1" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C522" s="1" t="s">
+        <v>1833</v>
+      </c>
+      <c r="E522" s="1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="F522" s="1" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="523" spans="1:6">
+      <c r="A523" s="1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C523" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="E523" s="1" t="s">
+        <v>1837</v>
+      </c>
+      <c r="F523" s="1" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="524" spans="1:6">
+      <c r="A524" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C524" s="1" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E524" s="1" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F524" s="1" t="s">
+        <v>1867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>